<commit_message>
Add option for >342 MUAC
</commit_message>
<xml_diff>
--- a/app/config/tables/GRAVIDA_VISIT/forms/GRAVIDA_VISIT/GRAVIDA_VISIT.xlsx
+++ b/app/config/tables/GRAVIDA_VISIT/forms/GRAVIDA_VISIT/GRAVIDA_VISIT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB85AA-55FC-44E3-B499-A19EDCB5E884}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34D0102-B852-4590-8306-4C06E91125BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="282">
   <si>
     <t>setting_name</t>
   </si>
@@ -862,6 +862,21 @@
   </si>
   <si>
     <t>{PREGID: opendatakit.getCurrentInstanceId(), REGID: data('REGID'), REGDIA: data('PREGDIA'), OUTDATE: data('OUTDATE'), ASSISTPART: data('ASSISTPART'), CART_ANC: data('CART_ANC'), CDG_C: data('CDG_C'), CDG_M: data('CDG_M'), FEDEP_C: data('FEDEP_C'), FEDEP_M: data('FEDEP_M'), GRCONS: data('GRCONS'), GRINFOS: data('GRINFOS'), GRVAC: data('GRVAC'), LITTERSIZE: data('LITTERSIZE'), LOCPAR: data('LOCPAR'), QVFANSI_C: data('QVFANSI_C'), QVFANSI_M: data('QVFANSI_M'), TABPART: data('TABPART'), VACTTHI: data('VACTTHI')}</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>muac</t>
+  </si>
+  <si>
+    <t>muacbig</t>
+  </si>
+  <si>
+    <t>More than 342 cm</t>
+  </si>
+  <si>
+    <t>data('muacbig') != null</t>
   </si>
 </sst>
 </file>
@@ -1393,11 +1408,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:I147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,283 +1516,278 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>13</v>
+      <c r="D8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" t="s">
+        <v>278</v>
+      </c>
+      <c r="F8" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="D12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>166</v>
-      </c>
-      <c r="F12" t="s">
-        <v>260</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="D17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
         <v>25</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E26" t="s">
         <v>50</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F26" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F29" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
+      <c r="G32" s="6"/>
+      <c r="H32" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>131</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F33" t="s">
         <v>55</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G33" t="s">
         <v>101</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C34" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" t="s">
-        <v>100</v>
-      </c>
-      <c r="H30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" t="s">
-        <v>103</v>
-      </c>
-      <c r="H34" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" t="s">
-        <v>43</v>
+      <c r="B37" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>13</v>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>12</v>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" t="s">
-        <v>45</v>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -1785,59 +1795,61 @@
         <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" t="s">
-        <v>61</v>
-      </c>
-      <c r="G44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H44" t="s">
-        <v>43</v>
+      <c r="B44" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>13</v>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" t="s">
+        <v>104</v>
+      </c>
+      <c r="H46" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>12</v>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6" t="s">
-        <v>46</v>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1845,197 +1857,192 @@
         <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G51" t="s">
-        <v>100</v>
-      </c>
-      <c r="H51" t="s">
-        <v>43</v>
+      <c r="B51" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>13</v>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" t="s">
-        <v>102</v>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" t="s">
+        <v>101</v>
+      </c>
+      <c r="H54" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>12</v>
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="F56" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="G56" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" t="s">
+        <v>59</v>
+      </c>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="B60" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="16"/>
+      <c r="B65" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C65" s="13" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="D62" t="s">
-        <v>25</v>
-      </c>
-      <c r="E62" t="s">
-        <v>142</v>
-      </c>
-      <c r="F62" t="s">
-        <v>143</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="D65" t="s">
-        <v>131</v>
-      </c>
-      <c r="F65" t="s">
-        <v>145</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
-      <c r="B67" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" t="s">
-        <v>147</v>
+      <c r="B67" s="11"/>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67" t="s">
+        <v>143</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="D69" t="s">
-        <v>30</v>
-      </c>
-      <c r="F69" t="s">
-        <v>148</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>149</v>
+      <c r="B69" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
-      <c r="B70" s="11" t="s">
-        <v>13</v>
+      <c r="B70" s="11"/>
+      <c r="D70" t="s">
+        <v>131</v>
+      </c>
+      <c r="F70" t="s">
+        <v>145</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2044,7 +2051,7 @@
         <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2060,13 +2067,13 @@
         <v>30</v>
       </c>
       <c r="F74" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2084,258 +2091,254 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="11" t="s">
-        <v>12</v>
+        <v>94</v>
+      </c>
+      <c r="C77" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="D78" t="s">
-        <v>25</v>
-      </c>
-      <c r="E78" t="s">
-        <v>153</v>
-      </c>
-      <c r="F78" t="s">
-        <v>153</v>
-      </c>
-      <c r="G78" t="s">
-        <v>154</v>
-      </c>
-      <c r="H78" t="s">
-        <v>155</v>
+      <c r="B78" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
-      <c r="B79" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C79" t="s">
-        <v>156</v>
+      <c r="B79" s="11"/>
+      <c r="D79" t="s">
+        <v>30</v>
+      </c>
+      <c r="F79" t="s">
+        <v>151</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="D80" t="s">
-        <v>25</v>
-      </c>
-      <c r="E80" t="s">
-        <v>157</v>
-      </c>
-      <c r="F80" t="s">
-        <v>157</v>
-      </c>
-      <c r="G80" t="s">
-        <v>158</v>
-      </c>
-      <c r="H80" t="s">
-        <v>159</v>
+      <c r="B80" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="11" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="D83" t="s">
-        <v>161</v>
+        <v>25</v>
+      </c>
+      <c r="E83" t="s">
+        <v>153</v>
       </c>
       <c r="F83" t="s">
-        <v>162</v>
-      </c>
-      <c r="I83" t="s">
-        <v>163</v>
+        <v>153</v>
+      </c>
+      <c r="G83" t="s">
+        <v>154</v>
+      </c>
+      <c r="H83" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="11" t="s">
-        <v>164</v>
+        <v>94</v>
+      </c>
+      <c r="C84" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
       <c r="D85" t="s">
-        <v>161</v>
+        <v>25</v>
+      </c>
+      <c r="E85" t="s">
+        <v>157</v>
       </c>
       <c r="F85" t="s">
-        <v>162</v>
-      </c>
-      <c r="I85" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+      <c r="G85" t="s">
+        <v>158</v>
+      </c>
+      <c r="H85" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="11" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="11" t="s">
-        <v>13</v>
+        <v>94</v>
+      </c>
+      <c r="C87" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
-      <c r="B88" s="11" t="s">
-        <v>12</v>
+      <c r="B88" s="11"/>
+      <c r="D88" t="s">
+        <v>161</v>
+      </c>
+      <c r="F88" t="s">
+        <v>162</v>
+      </c>
+      <c r="I88" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
-      <c r="D89" t="s">
-        <v>25</v>
-      </c>
-      <c r="E89" t="s">
-        <v>166</v>
-      </c>
-      <c r="F89" t="s">
-        <v>167</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>168</v>
+      <c r="B89" s="11" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
-      <c r="B90" s="11" t="s">
-        <v>13</v>
+      <c r="B90" s="11"/>
+      <c r="D90" t="s">
+        <v>161</v>
+      </c>
+      <c r="F90" t="s">
+        <v>162</v>
+      </c>
+      <c r="I90" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="11"/>
       <c r="B91" s="11" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
-      <c r="B92" s="11"/>
-      <c r="D92" t="s">
-        <v>25</v>
-      </c>
-      <c r="E92" t="s">
-        <v>50</v>
-      </c>
-      <c r="F92" t="s">
-        <v>169</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H92" s="6" t="s">
-        <v>100</v>
+      <c r="B92" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
-      <c r="B94" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="D94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" t="s">
+        <v>166</v>
+      </c>
+      <c r="F94" t="s">
+        <v>167</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="11"/>
-      <c r="B95" s="11"/>
-      <c r="D95" t="s">
-        <v>25</v>
-      </c>
-      <c r="E95" t="s">
-        <v>166</v>
-      </c>
-      <c r="F95" t="s">
-        <v>170</v>
-      </c>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6" t="s">
-        <v>171</v>
+      <c r="B95" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="11"/>
       <c r="B96" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C96" t="s">
-        <v>172</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>
       <c r="B97" s="11"/>
       <c r="D97" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="E97" t="s">
+        <v>50</v>
       </c>
       <c r="F97" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
       <c r="B98" s="11" t="s">
-        <v>96</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
       <c r="B99" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
-      <c r="B100" s="11" t="s">
-        <v>12</v>
+      <c r="B100" s="11"/>
+      <c r="D100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>166</v>
+      </c>
+      <c r="F100" t="s">
+        <v>170</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="D101" t="s">
-        <v>28</v>
-      </c>
-      <c r="G101" t="s">
-        <v>103</v>
-      </c>
-      <c r="H101" t="s">
-        <v>47</v>
+      <c r="B101" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C101" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -2345,69 +2348,69 @@
         <v>30</v>
       </c>
       <c r="F102" t="s">
-        <v>175</v>
-      </c>
-      <c r="G102" t="s">
-        <v>101</v>
-      </c>
-      <c r="H102" t="s">
-        <v>44</v>
+        <v>173</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="11"/>
       <c r="B103" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="11"/>
-      <c r="B104" s="11"/>
-      <c r="D104" t="s">
-        <v>30</v>
-      </c>
-      <c r="F104" t="s">
-        <v>177</v>
-      </c>
-      <c r="G104" t="s">
-        <v>100</v>
-      </c>
-      <c r="H104" t="s">
-        <v>43</v>
+      <c r="B104" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
       <c r="B105" s="11" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="11"/>
-      <c r="B106" s="11" t="s">
-        <v>13</v>
+      <c r="B106" s="11"/>
+      <c r="D106" t="s">
+        <v>28</v>
+      </c>
+      <c r="G106" t="s">
+        <v>103</v>
+      </c>
+      <c r="H106" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="11"/>
-      <c r="B107" s="11" t="s">
-        <v>12</v>
+      <c r="B107" s="11"/>
+      <c r="D107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" t="s">
+        <v>175</v>
+      </c>
+      <c r="G107" t="s">
+        <v>101</v>
+      </c>
+      <c r="H107" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="D108" t="s">
-        <v>28</v>
-      </c>
-      <c r="G108" t="s">
-        <v>104</v>
-      </c>
-      <c r="H108" t="s">
-        <v>45</v>
+      <c r="B108" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C108" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -2417,67 +2420,69 @@
         <v>30</v>
       </c>
       <c r="F109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G109" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H109" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="11"/>
       <c r="B110" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C110" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="11"/>
-      <c r="B111" s="11"/>
-      <c r="D111" t="s">
-        <v>30</v>
-      </c>
-      <c r="F111" t="s">
-        <v>179</v>
-      </c>
-      <c r="G111" t="s">
-        <v>100</v>
-      </c>
-      <c r="H111" t="s">
-        <v>43</v>
+      <c r="B111" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="11"/>
       <c r="B112" s="11" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="11"/>
-      <c r="B113" s="11" t="s">
-        <v>13</v>
+      <c r="B113" s="11"/>
+      <c r="D113" t="s">
+        <v>28</v>
+      </c>
+      <c r="G113" t="s">
+        <v>104</v>
+      </c>
+      <c r="H113" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="11"/>
-      <c r="B114" s="11" t="s">
-        <v>12</v>
+      <c r="B114" s="11"/>
+      <c r="D114" t="s">
+        <v>30</v>
+      </c>
+      <c r="F114" t="s">
+        <v>178</v>
+      </c>
+      <c r="G114" t="s">
+        <v>101</v>
+      </c>
+      <c r="H114" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="11"/>
-      <c r="B115" s="11"/>
-      <c r="D115" t="s">
-        <v>28</v>
-      </c>
-      <c r="G115" s="6"/>
-      <c r="H115" s="6" t="s">
-        <v>46</v>
+      <c r="B115" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C115" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,189 +2492,183 @@
         <v>30</v>
       </c>
       <c r="F116" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H116" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="11"/>
       <c r="B117" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C117" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="D118" t="s">
-        <v>30</v>
-      </c>
-      <c r="F118" t="s">
-        <v>181</v>
-      </c>
-      <c r="G118" t="s">
-        <v>100</v>
-      </c>
-      <c r="H118" t="s">
-        <v>43</v>
+      <c r="B118" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="11"/>
       <c r="B119" s="11" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="11"/>
-      <c r="B120" s="11" t="s">
-        <v>13</v>
+      <c r="B120" s="11"/>
+      <c r="D120" t="s">
+        <v>28</v>
+      </c>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="11"/>
-      <c r="B121" s="11" t="s">
-        <v>12</v>
+      <c r="B121" s="11"/>
+      <c r="D121" t="s">
+        <v>30</v>
+      </c>
+      <c r="F121" t="s">
+        <v>180</v>
+      </c>
+      <c r="G121" t="s">
+        <v>101</v>
+      </c>
+      <c r="H121" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
-      <c r="D122" t="s">
-        <v>25</v>
-      </c>
-      <c r="E122" t="s">
-        <v>166</v>
-      </c>
-      <c r="F122" t="s">
-        <v>182</v>
-      </c>
-      <c r="G122" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="H122" s="6" t="s">
-        <v>183</v>
+      <c r="B122" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C122" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="11"/>
-      <c r="B123" s="11" t="s">
-        <v>13</v>
+      <c r="B123" s="11"/>
+      <c r="D123" t="s">
+        <v>30</v>
+      </c>
+      <c r="F123" t="s">
+        <v>181</v>
+      </c>
+      <c r="G123" t="s">
+        <v>100</v>
+      </c>
+      <c r="H123" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="11"/>
       <c r="B124" s="11" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="11"/>
-      <c r="B125" s="11"/>
-      <c r="D125" t="s">
-        <v>25</v>
-      </c>
-      <c r="E125" t="s">
-        <v>184</v>
-      </c>
-      <c r="F125" t="s">
-        <v>185</v>
-      </c>
-      <c r="G125" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H125" s="6" t="s">
-        <v>186</v>
+      <c r="B125" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="11"/>
       <c r="B126" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="11"/>
-      <c r="B127" s="11" t="s">
-        <v>12</v>
+      <c r="B127" s="11"/>
+      <c r="D127" t="s">
+        <v>25</v>
+      </c>
+      <c r="E127" t="s">
+        <v>166</v>
+      </c>
+      <c r="F127" t="s">
+        <v>182</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="D128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E128" t="s">
-        <v>187</v>
-      </c>
-      <c r="F128" t="s">
-        <v>188</v>
-      </c>
-      <c r="G128" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="H128" s="6" t="s">
-        <v>189</v>
+      <c r="B128" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="11"/>
       <c r="B129" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G129" s="11"/>
-      <c r="H129" s="11"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="11"/>
-      <c r="B130" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C130" t="s">
-        <v>266</v>
-      </c>
-      <c r="G130" s="11"/>
-      <c r="H130" s="11"/>
+      <c r="B130" s="11"/>
+      <c r="D130" t="s">
+        <v>25</v>
+      </c>
+      <c r="E130" t="s">
+        <v>184</v>
+      </c>
+      <c r="F130" t="s">
+        <v>185</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H130" s="6" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="11"/>
       <c r="B131" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G131" s="11"/>
-      <c r="H131" s="11"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>
-      <c r="B132" s="11"/>
-      <c r="D132" t="s">
-        <v>28</v>
-      </c>
-      <c r="G132" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="H132" s="6" t="s">
-        <v>274</v>
+      <c r="B132" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="11"/>
       <c r="B133" s="11"/>
       <c r="D133" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="E133" t="s">
-        <v>267</v>
-      </c>
-      <c r="G133" s="11"/>
+        <v>187</v>
+      </c>
+      <c r="F133" t="s">
+        <v>188</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H133" s="6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="11"/>
@@ -2685,7 +2684,7 @@
         <v>94</v>
       </c>
       <c r="C135" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
@@ -2705,10 +2704,10 @@
         <v>28</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -2721,7 +2720,6 @@
         <v>267</v>
       </c>
       <c r="G138" s="11"/>
-      <c r="H138" s="11"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="11"/>
@@ -2734,19 +2732,71 @@
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="11"/>
       <c r="B140" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C140" t="s">
+        <v>268</v>
       </c>
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
+      <c r="A141" s="11"/>
+      <c r="B141" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G141" s="11"/>
+      <c r="H141" s="11"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
+      <c r="D142" t="s">
+        <v>28</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H142" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
+      <c r="D143" t="s">
+        <v>119</v>
+      </c>
+      <c r="E143" t="s">
+        <v>267</v>
+      </c>
+      <c r="G143" s="11"/>
+      <c r="H143" s="11"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="11"/>
+      <c r="B144" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G144" s="11"/>
+      <c r="H144" s="11"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="11"/>
+      <c r="B145" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="16"/>
-      <c r="B142" t="s">
+      <c r="G145" s="11"/>
+      <c r="H145" s="11"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="16"/>
+      <c r="B147" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2968,11 +3018,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:D23"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3652,6 +3702,21 @@
         <v>254</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>278</v>
+      </c>
+      <c r="B47" t="str">
+        <f>"555"</f>
+        <v>555</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3663,8 +3728,8 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add max LITTERSIZE: 4
</commit_message>
<xml_diff>
--- a/app/config/tables/GRAVIDA_VISIT/forms/GRAVIDA_VISIT/GRAVIDA_VISIT.xlsx
+++ b/app/config/tables/GRAVIDA_VISIT/forms/GRAVIDA_VISIT/GRAVIDA_VISIT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34D0102-B852-4590-8306-4C06E91125BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC8A368-ADA7-4B59-940E-53F0A55870F0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="288">
   <si>
     <t>setting_name</t>
   </si>
@@ -877,6 +877,24 @@
   </si>
   <si>
     <t>data('muacbig') != null</t>
+  </si>
+  <si>
+    <t>data('LITTERSIZE') &gt;='3'</t>
+  </si>
+  <si>
+    <t>data('LITTERSIZE') &gt;='4'</t>
+  </si>
+  <si>
+    <t>Registro da 3ª criança</t>
+  </si>
+  <si>
+    <t>Registration of 3th child</t>
+  </si>
+  <si>
+    <t>Registration of 4th child</t>
+  </si>
+  <si>
+    <t>Registro da 4ª criança</t>
   </si>
 </sst>
 </file>
@@ -1408,11 +1426,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,19 +2802,139 @@
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="11"/>
       <c r="B145" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="C145" t="s">
+        <v>282</v>
       </c>
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
+      <c r="A146" s="11"/>
+      <c r="B146" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G146" s="11"/>
+      <c r="H146" s="11"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="11"/>
+      <c r="B147" s="11"/>
+      <c r="D147" t="s">
+        <v>28</v>
+      </c>
+      <c r="G147" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H147" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="11"/>
+      <c r="B148" s="11"/>
+      <c r="D148" t="s">
+        <v>119</v>
+      </c>
+      <c r="E148" t="s">
+        <v>267</v>
+      </c>
+      <c r="G148" s="11"/>
+      <c r="H148" s="11"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="11"/>
+      <c r="B149" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G149" s="11"/>
+      <c r="H149" s="11"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="11"/>
+      <c r="B150" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C150" t="s">
+        <v>283</v>
+      </c>
+      <c r="G150" s="11"/>
+      <c r="H150" s="11"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="11"/>
+      <c r="B151" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" s="11"/>
+      <c r="H151" s="11"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="11"/>
+      <c r="B152" s="11"/>
+      <c r="D152" t="s">
+        <v>28</v>
+      </c>
+      <c r="G152" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="H152" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="11"/>
+      <c r="B153" s="11"/>
+      <c r="D153" t="s">
+        <v>119</v>
+      </c>
+      <c r="E153" t="s">
+        <v>267</v>
+      </c>
+      <c r="G153" s="11"/>
+      <c r="H153" s="11"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="11"/>
+      <c r="B154" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G154" s="11"/>
+      <c r="H154" s="11"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="11"/>
+      <c r="B155" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147" s="16"/>
-      <c r="B147" t="s">
+      <c r="G155" s="11"/>
+      <c r="H155" s="11"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="11"/>
+      <c r="B156" t="s">
+        <v>96</v>
+      </c>
+      <c r="G156" s="11"/>
+      <c r="H156" s="11"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="11"/>
+      <c r="B157" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G157" s="11"/>
+      <c r="H157" s="11"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="16"/>
+      <c r="B159" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3725,17 +3863,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4027,21 +4165,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>279</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>277</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>25</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -4049,10 +4187,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -4060,10 +4198,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -4071,7 +4209,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -4082,7 +4220,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -4093,7 +4231,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
@@ -4104,10 +4242,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4115,43 +4253,43 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" t="b">
+      <c r="C38" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -4159,7 +4297,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
         <v>130</v>
@@ -4168,9 +4306,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>265</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:C41">
-    <sortCondition ref="A39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>